<commit_message>
Uploaded 07-Apr-2021 14:12:27 {/src/main/resources/com/myspace/test/rule.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/test/rule.xlsx
+++ b/src/main/resources/com/myspace/test/rule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2307BDD-1664-41EC-8917-7EF9E3558A15}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07452AC-B43B-420E-9F00-53990AC3849B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="259" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1217,8 +1217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N1027"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1521,7 +1521,7 @@
       <c r="K11" s="19"/>
       <c r="L11" s="19"/>
       <c r="M11" s="23" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="N11" s="24"/>
     </row>

</xml_diff>

<commit_message>
Uploaded 07-Apr-2021 14:14:11 {/src/main/resources/com/myspace/test/rule.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/test/rule.xlsx
+++ b/src/main/resources/com/myspace/test/rule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07452AC-B43B-420E-9F00-53990AC3849B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50BC722-4B1D-4BDE-91F2-479CE6F69EA4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="259" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1217,8 +1217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N1027"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="I10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1521,7 +1521,7 @@
       <c r="K11" s="19"/>
       <c r="L11" s="19"/>
       <c r="M11" s="23" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="N11" s="24"/>
     </row>
@@ -1616,7 +1616,7 @@
       <c r="L15" s="21"/>
       <c r="M15" s="25"/>
       <c r="N15" s="24" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Uploaded 07-Apr-2021 14:18:50 {/src/main/resources/com/myspace/test/rule.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/test/rule.xlsx
+++ b/src/main/resources/com/myspace/test/rule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC157FD-4E43-4CC4-90F0-895D5952CC24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41AF4823-4B98-4FA4-9B81-92B734C58D57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="259" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1217,8 +1217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N1027"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" topLeftCell="I34" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="N48" sqref="N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1616,7 +1616,7 @@
       <c r="L15" s="21"/>
       <c r="M15" s="25"/>
       <c r="N15" s="24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -2552,7 +2552,7 @@
       <c r="L48" s="20"/>
       <c r="M48" s="25"/>
       <c r="N48" s="24" t="s">
-        <v>86</v>
+        <v>157</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Uploaded 07-Apr-2021 14:25:06 {/src/main/resources/com/myspace/test/rule.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/test/rule.xlsx
+++ b/src/main/resources/com/myspace/test/rule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41AF4823-4B98-4FA4-9B81-92B734C58D57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A3C7D2-BC88-40C4-88F6-6DFF33D79029}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="259" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1217,8 +1217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N1027"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I34" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="N48" sqref="N48"/>
+    <sheetView tabSelected="1" topLeftCell="I29" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="O51" sqref="O51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Uploaded 07-Apr-2021 14:30:03 {/src/main/resources/com/myspace/test/rule.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/test/rule.xlsx
+++ b/src/main/resources/com/myspace/test/rule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A3C7D2-BC88-40C4-88F6-6DFF33D79029}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFDE9D9-8F28-4F55-90A6-A47E85C4BFA4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="259" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1217,7 +1217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N1027"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I29" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="O51" sqref="O51"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Uploaded 07-Apr-2021 16:21:59 {/src/main/resources/com/myspace/test/rule.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/test/rule.xlsx
+++ b/src/main/resources/com/myspace/test/rule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFDE9D9-8F28-4F55-90A6-A47E85C4BFA4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57A4BFF-B250-4B64-B979-CA322AF4C026}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="259" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1217,7 +1217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N1027"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I37" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="O51" sqref="O51"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Uploaded 07-Apr-2021 17:54:25 {/src/main/resources/com/myspace/test/rule.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/test/rule.xlsx
+++ b/src/main/resources/com/myspace/test/rule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57A4BFF-B250-4B64-B979-CA322AF4C026}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C177D443-C3DA-4F94-B653-75AF4142C530}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="259" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1217,8 +1217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N1027"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I37" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="O51" sqref="O51"/>
+    <sheetView tabSelected="1" topLeftCell="I27" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="M50" sqref="M50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2552,7 +2552,7 @@
       <c r="L48" s="20"/>
       <c r="M48" s="25"/>
       <c r="N48" s="24" t="s">
-        <v>157</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Uploaded 07-Apr-2021 18:01:13 {/src/main/resources/com/myspace/test/rule.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/test/rule.xlsx
+++ b/src/main/resources/com/myspace/test/rule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C177D443-C3DA-4F94-B653-75AF4142C530}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{120D936D-77DE-49BF-8EAF-BF94A36A75F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="259" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1218,7 +1218,7 @@
   <dimension ref="A1:N1027"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I27" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="M50" sqref="M50"/>
+      <selection activeCell="N48" sqref="N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2552,7 +2552,7 @@
       <c r="L48" s="20"/>
       <c r="M48" s="25"/>
       <c r="N48" s="24" t="s">
-        <v>86</v>
+        <v>157</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Uploaded 07-Apr-2021 18:25:03 {/src/main/resources/com/myspace/test/rule.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/test/rule.xlsx
+++ b/src/main/resources/com/myspace/test/rule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{120D936D-77DE-49BF-8EAF-BF94A36A75F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6371DC-879F-411F-8B97-C1FC92019C2E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="259" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1217,8 +1217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N1027"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I27" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="N48" sqref="N48"/>
+    <sheetView tabSelected="1" topLeftCell="I43" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Uploaded 07-Apr-2021 18:26:21 {/src/main/resources/com/myspace/test/rule.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/test/rule.xlsx
+++ b/src/main/resources/com/myspace/test/rule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6371DC-879F-411F-8B97-C1FC92019C2E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9530100-D38C-4F56-A8C4-3723D0FB17A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="259" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1218,7 +1218,7 @@
   <dimension ref="A1:N1027"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I43" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:M1"/>
+      <selection activeCell="N48" sqref="N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2552,7 +2552,7 @@
       <c r="L48" s="20"/>
       <c r="M48" s="25"/>
       <c r="N48" s="24" t="s">
-        <v>157</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Uploaded 07-Apr-2021 18:55:00 {/src/main/resources/com/myspace/test/rule.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/test/rule.xlsx
+++ b/src/main/resources/com/myspace/test/rule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9530100-D38C-4F56-A8C4-3723D0FB17A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4E002B-C193-4F06-A764-CD48A34F5087}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="259" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2552,7 +2552,7 @@
       <c r="L48" s="20"/>
       <c r="M48" s="25"/>
       <c r="N48" s="24" t="s">
-        <v>86</v>
+        <v>157</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Uploaded 07-Apr-2021 18:57:39 {/src/main/resources/com/myspace/test/rule.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/test/rule.xlsx
+++ b/src/main/resources/com/myspace/test/rule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4E002B-C193-4F06-A764-CD48A34F5087}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1A8992-5338-4ADB-9F34-F98EE34208EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="259" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="170">
   <si>
     <t>RuleSet</t>
   </si>
@@ -531,6 +531,9 @@
   </si>
   <si>
     <t>com.myspace.test.Patient</t>
+  </si>
+  <si>
+    <t>General Followup(Ped follow up1)</t>
   </si>
 </sst>
 </file>
@@ -1217,8 +1220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N1027"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I43" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="N48" sqref="N48"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2555,97 +2558,133 @@
         <v>157</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B49" s="29"/>
-      <c r="C49" s="31"/>
-      <c r="F49" s="35"/>
-      <c r="G49" s="35"/>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B50" s="29"/>
-      <c r="C50" s="31"/>
-      <c r="F50" s="35"/>
-      <c r="G50" s="35"/>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A49" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="B49" s="28"/>
+      <c r="C49" s="28">
+        <v>18</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E49" s="20"/>
+      <c r="F49" s="34"/>
+      <c r="G49" s="34"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="20"/>
+      <c r="J49" s="20"/>
+      <c r="K49" s="20"/>
+      <c r="L49" s="20"/>
+      <c r="M49" s="25"/>
+      <c r="N49" s="24" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A50" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B50" s="28"/>
+      <c r="C50" s="28">
+        <v>18</v>
+      </c>
+      <c r="D50" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E50" s="20"/>
+      <c r="F50" s="34"/>
+      <c r="G50" s="34"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
+      <c r="J50" s="20"/>
+      <c r="K50" s="20"/>
+      <c r="L50" s="20"/>
+      <c r="M50" s="25"/>
+      <c r="N50" s="24" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B51" s="29"/>
       <c r="C51" s="31"/>
       <c r="F51" s="35"/>
       <c r="G51" s="35"/>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B52" s="29"/>
       <c r="C52" s="31"/>
       <c r="F52" s="35"/>
       <c r="G52" s="35"/>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B53" s="29"/>
       <c r="C53" s="31"/>
       <c r="F53" s="35"/>
       <c r="G53" s="35"/>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B54" s="29"/>
       <c r="C54" s="31"/>
       <c r="F54" s="35"/>
       <c r="G54" s="35"/>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B55" s="29"/>
       <c r="C55" s="31"/>
       <c r="F55" s="35"/>
       <c r="G55" s="35"/>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B56" s="29"/>
       <c r="C56" s="31"/>
       <c r="F56" s="35"/>
       <c r="G56" s="35"/>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B57" s="29"/>
       <c r="C57" s="31"/>
       <c r="F57" s="35"/>
       <c r="G57" s="35"/>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B58" s="29"/>
       <c r="C58" s="31"/>
       <c r="F58" s="35"/>
       <c r="G58" s="35"/>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B59" s="29"/>
       <c r="C59" s="31"/>
       <c r="F59" s="35"/>
       <c r="G59" s="35"/>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B60" s="29"/>
       <c r="C60" s="31"/>
       <c r="F60" s="35"/>
       <c r="G60" s="35"/>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B61" s="29"/>
       <c r="C61" s="31"/>
       <c r="F61" s="35"/>
       <c r="G61" s="35"/>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B62" s="29"/>
       <c r="C62" s="31"/>
       <c r="F62" s="35"/>
       <c r="G62" s="35"/>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B63" s="29"/>
       <c r="C63" s="31"/>
       <c r="F63" s="35"/>
       <c r="G63" s="35"/>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B64" s="29"/>
       <c r="C64" s="31"/>
       <c r="F64" s="35"/>
@@ -7666,10 +7705,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11:D1121 M11:M876" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"""Ancillary and Vaccination"",""Sick Visit"",""Pre-Op Clearance"",""Well Visit"",""General Follow Up"",""Adult Sick Visit"",""Medicare Sick Visit"",""Pediatric Sick Visit"",""Medicare Wellness Visit"",""Well Child Visit"",""Annual Physical Visit"""</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L11:L694 K11:K712 J11:J871" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J51:J871 L11:L694 J11:K50 K51:K712" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F11:I48" xr:uid="{FDB25CDC-1A47-40E7-9CE9-F1E87EFBC655}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F11:I50" xr:uid="{FDB25CDC-1A47-40E7-9CE9-F1E87EFBC655}">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Uploaded 07-Apr-2021 18:58:42 {/src/main/resources/com/myspace/test/rule.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/test/rule.xlsx
+++ b/src/main/resources/com/myspace/test/rule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1A8992-5338-4ADB-9F34-F98EE34208EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A670A7F7-2614-44DC-9FD6-25CAEA7AF594}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="259" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="170">
   <si>
     <t>RuleSet</t>
   </si>
@@ -1221,7 +1221,7 @@
   <dimension ref="A1:N1027"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2583,16 +2583,10 @@
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A50" s="20" t="s">
-        <v>85</v>
-      </c>
+      <c r="A50" s="20"/>
       <c r="B50" s="28"/>
-      <c r="C50" s="28">
-        <v>18</v>
-      </c>
-      <c r="D50" s="21" t="s">
-        <v>92</v>
-      </c>
+      <c r="C50" s="28"/>
+      <c r="D50" s="21"/>
       <c r="E50" s="20"/>
       <c r="F50" s="34"/>
       <c r="G50" s="34"/>
@@ -2602,9 +2596,7 @@
       <c r="K50" s="20"/>
       <c r="L50" s="20"/>
       <c r="M50" s="25"/>
-      <c r="N50" s="24" t="s">
-        <v>157</v>
-      </c>
+      <c r="N50" s="24"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B51" s="29"/>

</xml_diff>

<commit_message>
Uploaded 09-Apr-2021 16:43:33 {/src/main/resources/com/myspace/test/rule.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/test/rule.xlsx
+++ b/src/main/resources/com/myspace/test/rule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A670A7F7-2614-44DC-9FD6-25CAEA7AF594}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1B2C25-89A5-4E0F-A470-EB8EC351DD87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="259" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="169">
   <si>
     <t>RuleSet</t>
   </si>
@@ -531,9 +531,6 @@
   </si>
   <si>
     <t>com.myspace.test.Patient</t>
-  </si>
-  <si>
-    <t>General Followup(Ped follow up1)</t>
   </si>
 </sst>
 </file>
@@ -1218,10 +1215,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N1027"/>
+  <dimension ref="A1:N1026"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="I43" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="N48" sqref="N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2555,20 +2552,14 @@
       <c r="L48" s="20"/>
       <c r="M48" s="25"/>
       <c r="N48" s="24" t="s">
-        <v>157</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A49" s="20" t="s">
-        <v>169</v>
-      </c>
+      <c r="A49" s="20"/>
       <c r="B49" s="28"/>
-      <c r="C49" s="28">
-        <v>18</v>
-      </c>
-      <c r="D49" s="21" t="s">
-        <v>92</v>
-      </c>
+      <c r="C49" s="28"/>
+      <c r="D49" s="21"/>
       <c r="E49" s="20"/>
       <c r="F49" s="34"/>
       <c r="G49" s="34"/>
@@ -2578,25 +2569,13 @@
       <c r="K49" s="20"/>
       <c r="L49" s="20"/>
       <c r="M49" s="25"/>
-      <c r="N49" s="24" t="s">
-        <v>157</v>
-      </c>
+      <c r="N49" s="24"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A50" s="20"/>
-      <c r="B50" s="28"/>
-      <c r="C50" s="28"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="34"/>
-      <c r="G50" s="34"/>
-      <c r="H50" s="20"/>
-      <c r="I50" s="20"/>
-      <c r="J50" s="20"/>
-      <c r="K50" s="20"/>
-      <c r="L50" s="20"/>
-      <c r="M50" s="25"/>
-      <c r="N50" s="24"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="31"/>
+      <c r="F50" s="35"/>
+      <c r="G50" s="35"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B51" s="29"/>
@@ -6747,8 +6726,6 @@
     <row r="742" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B742" s="29"/>
       <c r="C742" s="31"/>
-      <c r="F742" s="35"/>
-      <c r="G742" s="35"/>
     </row>
     <row r="743" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B743" s="29"/>
@@ -7072,7 +7049,6 @@
     </row>
     <row r="823" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B823" s="29"/>
-      <c r="C823" s="31"/>
     </row>
     <row r="824" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B824" s="29"/>
@@ -7682,9 +7658,6 @@
     </row>
     <row r="1026" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1026" s="29"/>
-    </row>
-    <row r="1027" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1027" s="29"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -7694,13 +7667,13 @@
     <mergeCell ref="B8:L8"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11:D1121 M11:M876" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J50:J870 K50:K711 L11:L693 J11:K49" xr:uid="{00000000-0002-0000-0000-000001000000}">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11:D1120 M11:M875" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"""Ancillary and Vaccination"",""Sick Visit"",""Pre-Op Clearance"",""Well Visit"",""General Follow Up"",""Adult Sick Visit"",""Medicare Sick Visit"",""Pediatric Sick Visit"",""Medicare Wellness Visit"",""Well Child Visit"",""Annual Physical Visit"""</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J51:J871 L11:L694 J11:K50 K51:K712" xr:uid="{00000000-0002-0000-0000-000001000000}">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F11:I50" xr:uid="{FDB25CDC-1A47-40E7-9CE9-F1E87EFBC655}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F11:I49" xr:uid="{FDB25CDC-1A47-40E7-9CE9-F1E87EFBC655}">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
@@ -7718,13 +7691,13 @@
           <x14:formula1>
             <xm:f>'Dropdown List'!$A$2:$A$55</xm:f>
           </x14:formula1>
-          <xm:sqref>E11:E933</xm:sqref>
+          <xm:sqref>E11:E932</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>'Dropdown List'!$C$2:$C$35</xm:f>
           </x14:formula1>
-          <xm:sqref>N11:N901</xm:sqref>
+          <xm:sqref>N11:N900</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Uploaded 09-Apr-2021 16:45:48 {/src/main/resources/com/myspace/test/rule.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/test/rule.xlsx
+++ b/src/main/resources/com/myspace/test/rule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1B2C25-89A5-4E0F-A470-EB8EC351DD87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA9E7491-47BE-44A1-9F36-34FFFB3D12AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="259" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2552,7 +2552,7 @@
       <c r="L48" s="20"/>
       <c r="M48" s="25"/>
       <c r="N48" s="24" t="s">
-        <v>86</v>
+        <v>157</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>